<commit_message>
Mobile testing Check list
</commit_message>
<xml_diff>
--- a/Mobile testing check list.xlsx
+++ b/Mobile testing check list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Мой диск\QA\Mobile testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qa\group33\GitHub\Terminal\mobile_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C737860-73A4-48C0-8554-8E258F2D51B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E89977E-3315-4106-9F03-93480E19ED1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="297">
   <si>
     <t>№</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>Получить входящее сообщение из мессенджера, напоминания календаря</t>
-  </si>
-  <si>
-    <t>Перевести устройство в спящий режим/вывести из спящего режима</t>
   </si>
   <si>
     <t>Проверить правильность работы приложения при встряхивании 
@@ -215,15 +212,6 @@
 блокируют отдельные порты.</t>
   </si>
   <si>
-    <t>Huawei P8 lite 2017</t>
-  </si>
-  <si>
-    <t>Android 8.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android </t>
-  </si>
-  <si>
     <t>Открыть приложение, которому требуется доступ в интернет, без доступа в интернет</t>
   </si>
   <si>
@@ -360,10 +348,6 @@
     <t>Уведомление о низком заряде батареи/ аккумулятор полностью заряжен</t>
   </si>
   <si>
-    <t>Проверить взаимодействие  с GPS сенсором (при его включении/выключении, 
-использовании геолокационных данных)?</t>
-  </si>
-  <si>
     <t>Получить напоминание об обновлении приложения</t>
   </si>
   <si>
@@ -945,11 +929,16 @@
     <t>17.5</t>
   </si>
   <si>
-    <t>Правильность работы приложения, если устройство 
-находится в режиме "авиа" (это реконнект)</t>
-  </si>
-  <si>
     <t>Авиа режим</t>
+  </si>
+  <si>
+    <t>Iphone 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iOS 16.03.2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iOS </t>
   </si>
 </sst>
 </file>
@@ -1515,6 +1504,78 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1524,15 +1585,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1542,15 +1594,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1559,60 +1602,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1903,10 +1892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G259"/>
+  <dimension ref="A1:G256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129:A153"/>
+    <sheetView tabSelected="1" topLeftCell="A237" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,51 +1910,51 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="44" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="46" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>59</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>61</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="46" t="s">
-        <v>254</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>60</v>
+        <v>249</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C5" s="47"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="46" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="49" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C7" s="50">
         <v>44971</v>
@@ -1982,40 +1971,40 @@
         <v>0</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="57"/>
+      <c r="A10" s="79" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="81"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="69"/>
+      <c r="A11" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="87"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
@@ -2058,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2094,7 +2083,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2106,7 +2095,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2118,7 +2107,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2130,7 +2119,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2142,7 +2131,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2150,21 +2139,21 @@
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
-        <v>273</v>
-      </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="60"/>
+      <c r="A23" s="76" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" s="77"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="78"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="31">
         <v>12</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -2174,7 +2163,7 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="31"/>
       <c r="B25" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
@@ -2183,10 +2172,10 @@
     </row>
     <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
@@ -2195,10 +2184,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -2207,10 +2196,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
@@ -2219,10 +2208,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -2231,10 +2220,10 @@
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -2243,10 +2232,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
@@ -2255,10 +2244,10 @@
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -2267,10 +2256,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -2279,10 +2268,10 @@
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
@@ -2294,7 +2283,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
@@ -2304,7 +2293,7 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="31"/>
       <c r="B36" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
@@ -2313,10 +2302,10 @@
     </row>
     <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
@@ -2325,10 +2314,10 @@
     </row>
     <row r="38" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
@@ -2337,10 +2326,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
@@ -2349,10 +2338,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
@@ -2361,10 +2350,10 @@
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
@@ -2373,10 +2362,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="33" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -2385,10 +2374,10 @@
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -2400,7 +2389,7 @@
         <v>14</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
@@ -2410,7 +2399,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
@@ -2419,10 +2408,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
@@ -2432,7 +2421,7 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
@@ -2441,10 +2430,10 @@
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
@@ -2456,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
@@ -2466,7 +2455,7 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
@@ -2475,10 +2464,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
@@ -2487,10 +2476,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="33" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
@@ -2498,21 +2487,21 @@
       <c r="F52" s="32"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="70" t="s">
-        <v>102</v>
-      </c>
-      <c r="B53" s="71"/>
-      <c r="C53" s="71"/>
-      <c r="D53" s="71"/>
-      <c r="E53" s="71"/>
-      <c r="F53" s="72"/>
+      <c r="A53" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="63"/>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
@@ -2524,7 +2513,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
@@ -2533,10 +2522,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="54" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
@@ -2545,10 +2534,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="54" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
@@ -2557,10 +2546,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="54" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -2569,10 +2558,10 @@
     </row>
     <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="54" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
@@ -2581,10 +2570,10 @@
     </row>
     <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="54" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -2596,7 +2585,7 @@
         <v>18</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -2608,7 +2597,7 @@
         <v>19</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
@@ -2620,7 +2609,7 @@
         <v>20</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -2628,21 +2617,21 @@
       <c r="F63" s="32"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="70" t="s">
-        <v>272</v>
-      </c>
-      <c r="B64" s="71"/>
-      <c r="C64" s="71"/>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
-      <c r="F64" s="72"/>
+      <c r="A64" s="61" t="s">
+        <v>267</v>
+      </c>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="63"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="31">
         <v>22</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
@@ -2654,7 +2643,7 @@
         <v>23</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
@@ -2666,7 +2655,7 @@
         <v>24</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
@@ -2678,7 +2667,7 @@
         <v>25</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
@@ -2686,21 +2675,21 @@
       <c r="F68" s="32"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="B69" s="77"/>
-      <c r="C69" s="77"/>
-      <c r="D69" s="77"/>
-      <c r="E69" s="77"/>
-      <c r="F69" s="78"/>
+      <c r="A69" s="64" t="s">
+        <v>202</v>
+      </c>
+      <c r="B69" s="65"/>
+      <c r="C69" s="65"/>
+      <c r="D69" s="65"/>
+      <c r="E69" s="65"/>
+      <c r="F69" s="66"/>
     </row>
     <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="31">
         <v>26</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
@@ -2712,7 +2701,7 @@
         <v>27</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
@@ -2724,7 +2713,7 @@
         <v>28</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
@@ -2736,7 +2725,7 @@
         <v>29</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
@@ -2748,7 +2737,7 @@
         <v>30</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
@@ -2760,7 +2749,7 @@
         <v>31</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
@@ -2772,7 +2761,7 @@
         <v>32</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
@@ -2780,21 +2769,21 @@
       <c r="F76" s="32"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="79" t="s">
-        <v>215</v>
-      </c>
-      <c r="B77" s="80"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="80"/>
-      <c r="E77" s="80"/>
-      <c r="F77" s="81"/>
+      <c r="A77" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="B77" s="68"/>
+      <c r="C77" s="68"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="69"/>
     </row>
     <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="31">
         <v>33</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
@@ -2806,7 +2795,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
@@ -2818,7 +2807,7 @@
         <v>35</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C80" s="14"/>
       <c r="D80" s="14"/>
@@ -2826,21 +2815,21 @@
       <c r="F80" s="32"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="76" t="s">
-        <v>219</v>
-      </c>
-      <c r="B81" s="77"/>
-      <c r="C81" s="77"/>
-      <c r="D81" s="77"/>
-      <c r="E81" s="77"/>
-      <c r="F81" s="78"/>
+      <c r="A81" s="64" t="s">
+        <v>214</v>
+      </c>
+      <c r="B81" s="65"/>
+      <c r="C81" s="65"/>
+      <c r="D81" s="65"/>
+      <c r="E81" s="65"/>
+      <c r="F81" s="66"/>
     </row>
     <row r="82" spans="1:6" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="31">
         <v>36</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C82" s="14"/>
       <c r="D82" s="14"/>
@@ -2852,7 +2841,7 @@
         <v>37</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C83" s="25"/>
       <c r="D83" s="25"/>
@@ -2864,7 +2853,7 @@
         <v>38</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C84" s="25"/>
       <c r="D84" s="25"/>
@@ -2876,7 +2865,7 @@
         <v>39</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C85" s="25"/>
       <c r="D85" s="25"/>
@@ -2888,7 +2877,7 @@
         <v>40</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C86" s="25"/>
       <c r="D86" s="25"/>
@@ -2896,21 +2885,21 @@
       <c r="F86" s="35"/>
     </row>
     <row r="87" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="82" t="s">
-        <v>227</v>
-      </c>
-      <c r="B87" s="83"/>
-      <c r="C87" s="83"/>
-      <c r="D87" s="83"/>
-      <c r="E87" s="83"/>
-      <c r="F87" s="84"/>
+      <c r="A87" s="70" t="s">
+        <v>222</v>
+      </c>
+      <c r="B87" s="71"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="71"/>
+      <c r="F87" s="72"/>
     </row>
     <row r="88" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="31">
         <v>41</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C88" s="25"/>
       <c r="D88" s="25"/>
@@ -2922,7 +2911,7 @@
         <v>42</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C89" s="25"/>
       <c r="D89" s="25"/>
@@ -2934,7 +2923,7 @@
         <v>43</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C90" s="25"/>
       <c r="D90" s="25"/>
@@ -2946,7 +2935,7 @@
         <v>44</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C91" s="25"/>
       <c r="D91" s="25"/>
@@ -2958,7 +2947,7 @@
         <v>45</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C92" s="25"/>
       <c r="D92" s="25"/>
@@ -2970,7 +2959,7 @@
         <v>46</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C93" s="25"/>
       <c r="D93" s="25"/>
@@ -2982,7 +2971,7 @@
         <v>47</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C94" s="25"/>
       <c r="D94" s="25"/>
@@ -2994,7 +2983,7 @@
         <v>48</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C95" s="25"/>
       <c r="D95" s="25"/>
@@ -3006,7 +2995,7 @@
         <v>49</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C96" s="25"/>
       <c r="D96" s="25"/>
@@ -3018,7 +3007,7 @@
         <v>50</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C97" s="25"/>
       <c r="D97" s="25"/>
@@ -3026,21 +3015,21 @@
       <c r="F97" s="35"/>
     </row>
     <row r="98" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="B98" s="77"/>
-      <c r="C98" s="77"/>
-      <c r="D98" s="77"/>
-      <c r="E98" s="77"/>
-      <c r="F98" s="78"/>
+      <c r="A98" s="64" t="s">
+        <v>226</v>
+      </c>
+      <c r="B98" s="65"/>
+      <c r="C98" s="65"/>
+      <c r="D98" s="65"/>
+      <c r="E98" s="65"/>
+      <c r="F98" s="66"/>
     </row>
     <row r="99" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="31">
         <v>51</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C99" s="25"/>
       <c r="D99" s="25"/>
@@ -3052,7 +3041,7 @@
         <v>52</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C100" s="25"/>
       <c r="D100" s="25"/>
@@ -3064,7 +3053,7 @@
         <v>53</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C101" s="25"/>
       <c r="D101" s="25"/>
@@ -3072,21 +3061,21 @@
       <c r="F101" s="35"/>
     </row>
     <row r="102" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="B102" s="77"/>
-      <c r="C102" s="77"/>
-      <c r="D102" s="77"/>
-      <c r="E102" s="77"/>
-      <c r="F102" s="78"/>
+      <c r="A102" s="64" t="s">
+        <v>230</v>
+      </c>
+      <c r="B102" s="65"/>
+      <c r="C102" s="65"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="65"/>
+      <c r="F102" s="66"/>
     </row>
     <row r="103" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="31">
         <v>54</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C103" s="25"/>
       <c r="D103" s="25"/>
@@ -3098,7 +3087,7 @@
         <v>55</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C104" s="25"/>
       <c r="D104" s="25"/>
@@ -3110,7 +3099,7 @@
         <v>56</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C105" s="25"/>
       <c r="D105" s="25"/>
@@ -3118,21 +3107,21 @@
       <c r="F105" s="35"/>
     </row>
     <row r="106" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="67" t="s">
+      <c r="A106" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="B106" s="68"/>
-      <c r="C106" s="68"/>
-      <c r="D106" s="68"/>
-      <c r="E106" s="68"/>
-      <c r="F106" s="69"/>
+      <c r="B106" s="86"/>
+      <c r="C106" s="86"/>
+      <c r="D106" s="86"/>
+      <c r="E106" s="86"/>
+      <c r="F106" s="87"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="26">
         <v>57</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -3144,7 +3133,7 @@
         <v>58</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -3176,21 +3165,21 @@
       <c r="F110" s="10"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="67" t="s">
-        <v>57</v>
-      </c>
-      <c r="B111" s="68"/>
-      <c r="C111" s="68"/>
-      <c r="D111" s="68"/>
-      <c r="E111" s="68"/>
-      <c r="F111" s="69"/>
+      <c r="A111" s="85" t="s">
+        <v>56</v>
+      </c>
+      <c r="B111" s="86"/>
+      <c r="C111" s="86"/>
+      <c r="D111" s="86"/>
+      <c r="E111" s="86"/>
+      <c r="F111" s="87"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="26">
         <v>58</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
@@ -3202,7 +3191,7 @@
         <v>59</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
@@ -3214,7 +3203,7 @@
         <v>60</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
@@ -3226,7 +3215,7 @@
         <v>61</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -3238,7 +3227,7 @@
         <v>62</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
@@ -3262,7 +3251,7 @@
         <v>65</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
@@ -3274,7 +3263,7 @@
         <v>66</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
@@ -3286,7 +3275,7 @@
         <v>67</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
@@ -3294,14 +3283,14 @@
       <c r="F120" s="10"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="61" t="s">
+      <c r="A121" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="B121" s="62"/>
-      <c r="C121" s="62"/>
-      <c r="D121" s="62"/>
-      <c r="E121" s="62"/>
-      <c r="F121" s="63"/>
+      <c r="B121" s="83"/>
+      <c r="C121" s="83"/>
+      <c r="D121" s="83"/>
+      <c r="E121" s="83"/>
+      <c r="F121" s="84"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="26">
@@ -3329,21 +3318,21 @@
       <c r="F123" s="10"/>
     </row>
     <row r="124" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="64" t="s">
-        <v>239</v>
-      </c>
-      <c r="B124" s="65"/>
-      <c r="C124" s="65"/>
-      <c r="D124" s="65"/>
-      <c r="E124" s="65"/>
-      <c r="F124" s="66"/>
+      <c r="A124" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="B124" s="56"/>
+      <c r="C124" s="56"/>
+      <c r="D124" s="56"/>
+      <c r="E124" s="56"/>
+      <c r="F124" s="57"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="36">
         <v>70</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C125" s="21"/>
       <c r="D125" s="21"/>
@@ -3355,7 +3344,7 @@
         <v>71</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C126" s="21"/>
       <c r="D126" s="21"/>
@@ -3363,24 +3352,24 @@
       <c r="F126" s="37"/>
     </row>
     <row r="127" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="64" t="s">
-        <v>150</v>
-      </c>
-      <c r="B127" s="65"/>
-      <c r="C127" s="65"/>
-      <c r="D127" s="65"/>
-      <c r="E127" s="65"/>
-      <c r="F127" s="66"/>
+      <c r="A127" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="B127" s="56"/>
+      <c r="C127" s="56"/>
+      <c r="D127" s="56"/>
+      <c r="E127" s="56"/>
+      <c r="F127" s="57"/>
     </row>
     <row r="128" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="61" t="s">
+      <c r="A128" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="B128" s="62"/>
-      <c r="C128" s="62"/>
-      <c r="D128" s="62"/>
-      <c r="E128" s="62"/>
-      <c r="F128" s="63"/>
+      <c r="B128" s="83"/>
+      <c r="C128" s="83"/>
+      <c r="D128" s="83"/>
+      <c r="E128" s="83"/>
+      <c r="F128" s="84"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="26">
@@ -3543,7 +3532,7 @@
         <v>85</v>
       </c>
       <c r="B142" s="41" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
@@ -3555,7 +3544,7 @@
         <v>86</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
@@ -3567,14 +3556,14 @@
         <v>87</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
       <c r="F144" s="10"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="26">
         <v>88</v>
       </c>
@@ -3591,19 +3580,19 @@
         <v>89</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="26">
         <v>90</v>
       </c>
-      <c r="B147" s="4" t="s">
-        <v>105</v>
+      <c r="B147" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
@@ -3615,7 +3604,7 @@
         <v>91</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
@@ -3627,239 +3616,239 @@
         <v>92</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>298</v>
+        <v>92</v>
       </c>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="26">
         <v>93</v>
       </c>
-      <c r="B150" s="18" t="s">
-        <v>104</v>
+      <c r="B150" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A151" s="26">
+    <row r="151" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A151" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151" s="77"/>
+      <c r="C151" s="77"/>
+      <c r="D151" s="77"/>
+      <c r="E151" s="77"/>
+      <c r="F151" s="78"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="26">
         <v>94</v>
       </c>
-      <c r="B151" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="10"/>
-    </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A152" s="26">
-        <v>95</v>
-      </c>
       <c r="B152" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="F152" s="10"/>
     </row>
-    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="26">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="F153" s="10"/>
     </row>
-    <row r="154" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A154" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="B154" s="59"/>
-      <c r="C154" s="59"/>
-      <c r="D154" s="59"/>
-      <c r="E154" s="59"/>
-      <c r="F154" s="60"/>
+    <row r="154" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="B154" s="77"/>
+      <c r="C154" s="77"/>
+      <c r="D154" s="77"/>
+      <c r="E154" s="77"/>
+      <c r="F154" s="78"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="26">
+      <c r="A155" s="31">
         <v>96</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C155" s="25"/>
+      <c r="D155" s="25"/>
+      <c r="E155" s="25"/>
+      <c r="F155" s="35"/>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="31">
+        <v>97</v>
+      </c>
+      <c r="B156" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C156" s="25"/>
+      <c r="D156" s="25"/>
+      <c r="E156" s="25"/>
+      <c r="F156" s="35"/>
+    </row>
+    <row r="157" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A157" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B157" s="86"/>
+      <c r="C157" s="86"/>
+      <c r="D157" s="86"/>
+      <c r="E157" s="86"/>
+      <c r="F157" s="87"/>
+    </row>
+    <row r="158" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="26">
         <v>98</v>
       </c>
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="10"/>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="26">
-        <v>97</v>
-      </c>
-      <c r="B156" s="4" t="s">
+      <c r="B158" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="10"/>
+    </row>
+    <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A159" s="26">
         <v>99</v>
       </c>
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2"/>
-      <c r="F156" s="10"/>
-    </row>
-    <row r="157" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="B157" s="59"/>
-      <c r="C157" s="59"/>
-      <c r="D157" s="59"/>
-      <c r="E157" s="59"/>
-      <c r="F157" s="60"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="31">
-        <v>98</v>
-      </c>
-      <c r="B158" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="C158" s="25"/>
-      <c r="D158" s="25"/>
-      <c r="E158" s="25"/>
-      <c r="F158" s="35"/>
-    </row>
-    <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A159" s="31">
-        <v>99</v>
-      </c>
-      <c r="B159" s="21" t="s">
-        <v>154</v>
-      </c>
-      <c r="C159" s="25"/>
-      <c r="D159" s="25"/>
-      <c r="E159" s="25"/>
-      <c r="F159" s="35"/>
-    </row>
-    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A160" s="67" t="s">
-        <v>15</v>
-      </c>
-      <c r="B160" s="68"/>
-      <c r="C160" s="68"/>
-      <c r="D160" s="68"/>
-      <c r="E160" s="68"/>
-      <c r="F160" s="69"/>
+      <c r="B159" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
+      <c r="F159" s="10"/>
+    </row>
+    <row r="160" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="26">
+        <v>100</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="10"/>
     </row>
     <row r="161" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="26">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="26">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="26">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="26">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
       <c r="F164" s="10"/>
     </row>
-    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A165" s="26">
-        <v>104</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
-      <c r="E165" s="2"/>
-      <c r="F165" s="10"/>
-    </row>
-    <row r="166" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" s="56"/>
+      <c r="C165" s="56"/>
+      <c r="D165" s="56"/>
+      <c r="E165" s="56"/>
+      <c r="F165" s="57"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="26">
         <v>105</v>
       </c>
-      <c r="B166" s="4" t="s">
-        <v>140</v>
+      <c r="B166" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
       <c r="F166" s="10"/>
     </row>
-    <row r="167" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="26">
         <v>106</v>
       </c>
-      <c r="B167" s="4" t="s">
-        <v>151</v>
+      <c r="B167" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="10"/>
     </row>
-    <row r="168" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B168" s="65"/>
-      <c r="C168" s="65"/>
-      <c r="D168" s="65"/>
-      <c r="E168" s="65"/>
-      <c r="F168" s="66"/>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="26">
+        <v>107</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="10"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="26">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
@@ -3868,10 +3857,10 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="26">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>114</v>
+        <v>33</v>
       </c>
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
@@ -3880,10 +3869,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="26">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -3892,10 +3881,10 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="26">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
@@ -3904,10 +3893,10 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="26">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
@@ -3916,10 +3905,10 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="26">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
@@ -3928,10 +3917,10 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="26">
+        <v>114</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
@@ -3940,116 +3929,116 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="26">
+        <v>115</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
       <c r="F176" s="10"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="26">
-        <v>115</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>36</v>
+        <v>116</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="10"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="26">
-        <v>116</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="10"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="26">
-        <v>117</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="10"/>
     </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="26">
-        <v>118</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C180" s="2"/>
-      <c r="D180" s="2"/>
-      <c r="E180" s="2"/>
-      <c r="F180" s="10"/>
+    <row r="180" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B180" s="56"/>
+      <c r="C180" s="56"/>
+      <c r="D180" s="56"/>
+      <c r="E180" s="56"/>
+      <c r="F180" s="57"/>
     </row>
     <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="26">
+      <c r="A181" s="38">
         <v>119</v>
       </c>
-      <c r="B181" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C181" s="2"/>
-      <c r="D181" s="2"/>
-      <c r="E181" s="2"/>
-      <c r="F181" s="10"/>
-    </row>
-    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B181" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C181" s="27"/>
+      <c r="D181" s="27"/>
+      <c r="E181" s="27"/>
+      <c r="F181" s="39"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="26">
         <v>120</v>
       </c>
-      <c r="B182" s="4" t="s">
-        <v>62</v>
+      <c r="B182" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="10"/>
     </row>
-    <row r="183" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="B183" s="65"/>
-      <c r="C183" s="65"/>
-      <c r="D183" s="65"/>
-      <c r="E183" s="65"/>
-      <c r="F183" s="66"/>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="38">
+        <v>121</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
+      <c r="E183" s="2"/>
+      <c r="F183" s="10"/>
     </row>
     <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" s="38">
-        <v>121</v>
-      </c>
-      <c r="B184" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C184" s="27"/>
-      <c r="D184" s="27"/>
-      <c r="E184" s="27"/>
-      <c r="F184" s="39"/>
+      <c r="A184" s="26">
+        <v>122</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="2"/>
+      <c r="F184" s="10"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A185" s="26">
-        <v>122</v>
+      <c r="A185" s="38">
+        <v>123</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
@@ -4057,23 +4046,23 @@
       <c r="F185" s="10"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A186" s="38">
-        <v>123</v>
+      <c r="A186" s="26">
+        <v>124</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>129</v>
+        <v>46</v>
       </c>
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
       <c r="F186" s="10"/>
     </row>
-    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A187" s="26">
-        <v>124</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>176</v>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="38">
+        <v>125</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
@@ -4081,11 +4070,11 @@
       <c r="F187" s="10"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A188" s="38">
-        <v>125</v>
+      <c r="A188" s="26">
+        <v>126</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
@@ -4093,47 +4082,47 @@
       <c r="F188" s="10"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A189" s="26">
-        <v>126</v>
+      <c r="A189" s="38">
+        <v>127</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
       <c r="F189" s="10"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="38">
-        <v>127</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>47</v>
+    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" s="26">
+        <v>128</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
       <c r="F190" s="10"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="26">
-        <v>128</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>48</v>
+    <row r="191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" s="38">
+        <v>129</v>
+      </c>
+      <c r="B191" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
       <c r="F191" s="10"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A192" s="38">
-        <v>129</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>49</v>
+    <row r="192" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A192" s="26">
+        <v>130</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
@@ -4141,11 +4130,11 @@
       <c r="F192" s="10"/>
     </row>
     <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A193" s="26">
-        <v>130</v>
+      <c r="A193" s="38">
+        <v>131</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
@@ -4153,10 +4142,10 @@
       <c r="F193" s="10"/>
     </row>
     <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A194" s="38">
-        <v>131</v>
-      </c>
-      <c r="B194" s="18" t="s">
+      <c r="A194" s="26">
+        <v>132</v>
+      </c>
+      <c r="B194" s="4" t="s">
         <v>121</v>
       </c>
       <c r="C194" s="2"/>
@@ -4165,11 +4154,11 @@
       <c r="F194" s="10"/>
     </row>
     <row r="195" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A195" s="26">
-        <v>132</v>
+      <c r="A195" s="38">
+        <v>133</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>275</v>
+        <v>54</v>
       </c>
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
@@ -4177,23 +4166,23 @@
       <c r="F195" s="10"/>
     </row>
     <row r="196" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="38">
-        <v>133</v>
+      <c r="A196" s="26">
+        <v>134</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A197" s="26">
-        <v>134</v>
+    <row r="197" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A197" s="38">
+        <v>135</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
@@ -4201,8 +4190,8 @@
       <c r="F197" s="10"/>
     </row>
     <row r="198" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A198" s="38">
-        <v>135</v>
+      <c r="A198" s="26">
+        <v>136</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>55</v>
@@ -4213,35 +4202,35 @@
       <c r="F198" s="10"/>
     </row>
     <row r="199" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A199" s="26">
-        <v>136</v>
+      <c r="A199" s="38">
+        <v>137</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
       <c r="F199" s="10"/>
     </row>
-    <row r="200" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A200" s="38">
-        <v>137</v>
+    <row r="200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A200" s="26">
+        <v>138</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
       <c r="F200" s="10"/>
     </row>
-    <row r="201" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A201" s="26">
-        <v>138</v>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" s="38">
+        <v>139</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
@@ -4249,8 +4238,8 @@
       <c r="F201" s="10"/>
     </row>
     <row r="202" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A202" s="38">
-        <v>139</v>
+      <c r="A202" s="26">
+        <v>140</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>122</v>
@@ -4260,21 +4249,21 @@
       <c r="E202" s="2"/>
       <c r="F202" s="10"/>
     </row>
-    <row r="203" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A203" s="26">
-        <v>140</v>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" s="38">
+        <v>141</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
       <c r="F203" s="10"/>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="38">
-        <v>141</v>
+    <row r="204" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A204" s="26">
+        <v>142</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>125</v>
@@ -4284,84 +4273,84 @@
       <c r="E204" s="2"/>
       <c r="F204" s="10"/>
     </row>
-    <row r="205" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A205" s="26">
-        <v>142</v>
+    <row r="205" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="38">
+        <v>143</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
       <c r="F205" s="10"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" s="38">
-        <v>143</v>
+    <row r="206" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A206" s="26">
+        <v>144</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
       <c r="F206" s="10"/>
     </row>
-    <row r="207" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A207" s="26">
-        <v>144</v>
+    <row r="207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A207" s="38">
+        <v>145</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
       <c r="F207" s="10"/>
     </row>
-    <row r="208" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="38">
-        <v>145</v>
+    <row r="208" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A208" s="26">
+        <v>146</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="10"/>
     </row>
-    <row r="209" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A209" s="26">
-        <v>146</v>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" s="38">
+        <v>147</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
       <c r="F209" s="10"/>
     </row>
-    <row r="210" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="38">
-        <v>147</v>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" s="26">
+        <v>148</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
       <c r="F210" s="10"/>
     </row>
-    <row r="211" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A211" s="26">
-        <v>148</v>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" s="38">
+        <v>149</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
@@ -4369,11 +4358,11 @@
       <c r="F211" s="10"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" s="38">
-        <v>149</v>
+      <c r="A212" s="26">
+        <v>150</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
@@ -4381,11 +4370,11 @@
       <c r="F212" s="10"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="26">
-        <v>150</v>
+      <c r="A213" s="38">
+        <v>151</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
@@ -4393,11 +4382,11 @@
       <c r="F213" s="10"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="38">
-        <v>151</v>
+      <c r="A214" s="26">
+        <v>152</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
@@ -4405,11 +4394,11 @@
       <c r="F214" s="10"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="26">
-        <v>152</v>
+      <c r="A215" s="38">
+        <v>153</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
@@ -4417,11 +4406,11 @@
       <c r="F215" s="10"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="38">
-        <v>153</v>
+      <c r="A216" s="26">
+        <v>154</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
@@ -4429,11 +4418,11 @@
       <c r="F216" s="10"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="26">
-        <v>154</v>
+      <c r="A217" s="38">
+        <v>155</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
@@ -4441,23 +4430,23 @@
       <c r="F217" s="10"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A218" s="38">
-        <v>155</v>
+      <c r="A218" s="26">
+        <v>156</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
       <c r="F218" s="10"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A219" s="26">
-        <v>156</v>
+    <row r="219" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A219" s="38">
+        <v>157</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>182</v>
+        <v>243</v>
       </c>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
@@ -4465,35 +4454,33 @@
       <c r="F219" s="10"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="38">
-        <v>157</v>
-      </c>
-      <c r="B220" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C220" s="2"/>
-      <c r="D220" s="2"/>
-      <c r="E220" s="2"/>
-      <c r="F220" s="10"/>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" s="73" t="s">
+        <v>244</v>
+      </c>
+      <c r="B220" s="74"/>
+      <c r="C220" s="74"/>
+      <c r="D220" s="74"/>
+      <c r="E220" s="74"/>
+      <c r="F220" s="75"/>
+    </row>
+    <row r="221" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="26">
         <v>158</v>
       </c>
-      <c r="B221" s="4" t="s">
-        <v>184</v>
+      <c r="B221" s="43" t="s">
+        <v>136</v>
       </c>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
       <c r="F221" s="10"/>
     </row>
-    <row r="222" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A222" s="38">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="26">
         <v>159</v>
       </c>
-      <c r="B222" s="4" t="s">
-        <v>248</v>
+      <c r="B222" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
@@ -4501,33 +4488,35 @@
       <c r="F222" s="10"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="B223" s="86"/>
-      <c r="C223" s="86"/>
-      <c r="D223" s="86"/>
-      <c r="E223" s="86"/>
-      <c r="F223" s="87"/>
-    </row>
-    <row r="224" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A223" s="26">
+        <v>160</v>
+      </c>
+      <c r="B223" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C223" s="2"/>
+      <c r="D223" s="2"/>
+      <c r="E223" s="2"/>
+      <c r="F223" s="10"/>
+    </row>
+    <row r="224" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="26">
-        <v>160</v>
-      </c>
-      <c r="B224" s="43" t="s">
-        <v>141</v>
+        <v>161</v>
+      </c>
+      <c r="B224" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
       <c r="F224" s="10"/>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A225" s="26">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B225" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
@@ -4536,118 +4525,118 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="26">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B226" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="10"/>
     </row>
-    <row r="227" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="26">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B227" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
       <c r="F227" s="10"/>
     </row>
-    <row r="228" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="26">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B228" s="28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
       <c r="F228" s="10"/>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="26">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B229" s="28" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
       <c r="F229" s="10"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="26">
-        <v>166</v>
-      </c>
-      <c r="B230" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C230" s="2"/>
-      <c r="D230" s="2"/>
-      <c r="E230" s="2"/>
-      <c r="F230" s="10"/>
-    </row>
-    <row r="231" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="26">
+    <row r="230" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B230" s="56"/>
+      <c r="C230" s="56"/>
+      <c r="D230" s="56"/>
+      <c r="E230" s="56"/>
+      <c r="F230" s="57"/>
+      <c r="G230" s="19"/>
+    </row>
+    <row r="231" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A231" s="31">
         <v>167</v>
       </c>
-      <c r="B231" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="C231" s="2"/>
-      <c r="D231" s="2"/>
-      <c r="E231" s="2"/>
-      <c r="F231" s="10"/>
-    </row>
-    <row r="232" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B231" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C231" s="25"/>
+      <c r="D231" s="25"/>
+      <c r="E231" s="25"/>
+      <c r="F231" s="35"/>
+      <c r="G231" s="19"/>
+    </row>
+    <row r="232" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="26">
         <v>168</v>
       </c>
       <c r="B232" s="28" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
       <c r="F232" s="10"/>
     </row>
-    <row r="233" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="64" t="s">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="31">
+        <v>169</v>
+      </c>
+      <c r="B233" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C233" s="2"/>
+      <c r="D233" s="2"/>
+      <c r="E233" s="2"/>
+      <c r="F233" s="10"/>
+    </row>
+    <row r="234" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A234" s="26">
+        <v>170</v>
+      </c>
+      <c r="B234" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C234" s="2"/>
+      <c r="D234" s="2"/>
+      <c r="E234" s="2"/>
+      <c r="F234" s="10"/>
+    </row>
+    <row r="235" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A235" s="31">
+        <v>171</v>
+      </c>
+      <c r="B235" s="29" t="s">
         <v>156</v>
-      </c>
-      <c r="B233" s="65"/>
-      <c r="C233" s="65"/>
-      <c r="D233" s="65"/>
-      <c r="E233" s="65"/>
-      <c r="F233" s="66"/>
-      <c r="G233" s="19"/>
-    </row>
-    <row r="234" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A234" s="31">
-        <v>169</v>
-      </c>
-      <c r="B234" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="C234" s="25"/>
-      <c r="D234" s="25"/>
-      <c r="E234" s="25"/>
-      <c r="F234" s="35"/>
-      <c r="G234" s="19"/>
-    </row>
-    <row r="235" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="26">
-        <v>170</v>
-      </c>
-      <c r="B235" s="28" t="s">
-        <v>157</v>
       </c>
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
@@ -4655,35 +4644,35 @@
       <c r="F235" s="10"/>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236" s="31">
-        <v>171</v>
+      <c r="A236" s="26">
+        <v>172</v>
       </c>
       <c r="B236" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
       <c r="F236" s="10"/>
     </row>
-    <row r="237" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A237" s="26">
-        <v>172</v>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" s="31">
+        <v>173</v>
       </c>
       <c r="B237" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
       <c r="F237" s="10"/>
     </row>
-    <row r="238" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A238" s="31">
-        <v>173</v>
-      </c>
-      <c r="B238" s="29" t="s">
-        <v>161</v>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="26">
+        <v>174</v>
+      </c>
+      <c r="B238" s="28" t="s">
+        <v>159</v>
       </c>
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
@@ -4691,11 +4680,11 @@
       <c r="F238" s="10"/>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A239" s="26">
-        <v>174</v>
+      <c r="A239" s="31">
+        <v>175</v>
       </c>
       <c r="B239" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
@@ -4703,105 +4692,103 @@
       <c r="F239" s="10"/>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A240" s="31">
-        <v>175</v>
+      <c r="A240" s="26">
+        <v>176</v>
       </c>
       <c r="B240" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
       <c r="F240" s="10"/>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" s="26">
-        <v>176</v>
-      </c>
-      <c r="B241" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="C241" s="2"/>
-      <c r="D241" s="2"/>
-      <c r="E241" s="2"/>
-      <c r="F241" s="10"/>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" s="31">
+    <row r="241" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B241" s="56"/>
+      <c r="C241" s="56"/>
+      <c r="D241" s="56"/>
+      <c r="E241" s="56"/>
+      <c r="F241" s="57"/>
+    </row>
+    <row r="242" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A242" s="26">
         <v>177</v>
       </c>
       <c r="B242" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
       <c r="F242" s="10"/>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A243" s="26">
         <v>178</v>
       </c>
       <c r="B243" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
       <c r="F243" s="10"/>
     </row>
-    <row r="244" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="64" t="s">
-        <v>167</v>
-      </c>
-      <c r="B244" s="65"/>
-      <c r="C244" s="65"/>
-      <c r="D244" s="65"/>
-      <c r="E244" s="65"/>
-      <c r="F244" s="66"/>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="26">
+        <v>179</v>
+      </c>
+      <c r="B244" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C244" s="2"/>
+      <c r="D244" s="2"/>
+      <c r="E244" s="2"/>
+      <c r="F244" s="10"/>
     </row>
     <row r="245" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="26">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B245" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
       <c r="F245" s="10"/>
     </row>
-    <row r="246" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="26">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B246" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
       <c r="F246" s="10"/>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" s="26">
-        <v>181</v>
-      </c>
-      <c r="B247" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="C247" s="2"/>
-      <c r="D247" s="2"/>
-      <c r="E247" s="2"/>
-      <c r="F247" s="10"/>
+    <row r="247" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="B247" s="59"/>
+      <c r="C247" s="59"/>
+      <c r="D247" s="59"/>
+      <c r="E247" s="59"/>
+      <c r="F247" s="60"/>
     </row>
     <row r="248" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="26">
         <v>182</v>
       </c>
       <c r="B248" s="28" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
@@ -4813,134 +4800,111 @@
         <v>183</v>
       </c>
       <c r="B249" s="28" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
       <c r="F249" s="10"/>
     </row>
-    <row r="250" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="73" t="s">
-        <v>185</v>
-      </c>
-      <c r="B250" s="74"/>
-      <c r="C250" s="74"/>
-      <c r="D250" s="74"/>
-      <c r="E250" s="74"/>
-      <c r="F250" s="75"/>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="26">
+        <v>184</v>
+      </c>
+      <c r="B250" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="C250" s="2"/>
+      <c r="D250" s="2"/>
+      <c r="E250" s="2"/>
+      <c r="F250" s="10"/>
     </row>
     <row r="251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="26">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B251" s="28" t="s">
-        <v>186</v>
+        <v>245</v>
       </c>
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
       <c r="F251" s="10"/>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" s="26">
-        <v>185</v>
-      </c>
-      <c r="B252" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="C252" s="2"/>
-      <c r="D252" s="2"/>
-      <c r="E252" s="2"/>
-      <c r="F252" s="10"/>
+    <row r="252" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="B252" s="56"/>
+      <c r="C252" s="56"/>
+      <c r="D252" s="56"/>
+      <c r="E252" s="56"/>
+      <c r="F252" s="57"/>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="26">
         <v>186</v>
       </c>
       <c r="B253" s="28" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
       <c r="F253" s="10"/>
     </row>
-    <row r="254" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="26">
         <v>187</v>
       </c>
       <c r="B254" s="28" t="s">
-        <v>250</v>
+        <v>186</v>
       </c>
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
       <c r="F254" s="10"/>
     </row>
-    <row r="255" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="64" t="s">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="26">
+        <v>188</v>
+      </c>
+      <c r="B255" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C255" s="2"/>
+      <c r="D255" s="2"/>
+      <c r="E255" s="2"/>
+      <c r="F255" s="10"/>
+    </row>
+    <row r="256" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A256" s="42">
         <v>189</v>
       </c>
-      <c r="B255" s="65"/>
-      <c r="C255" s="65"/>
-      <c r="D255" s="65"/>
-      <c r="E255" s="65"/>
-      <c r="F255" s="66"/>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A256" s="26">
+      <c r="B256" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="B256" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="C256" s="2"/>
-      <c r="D256" s="2"/>
-      <c r="E256" s="2"/>
-      <c r="F256" s="10"/>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A257" s="26">
-        <v>189</v>
-      </c>
-      <c r="B257" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="C257" s="2"/>
-      <c r="D257" s="2"/>
-      <c r="E257" s="2"/>
-      <c r="F257" s="10"/>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A258" s="26">
-        <v>190</v>
-      </c>
-      <c r="B258" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="C258" s="2"/>
-      <c r="D258" s="2"/>
-      <c r="E258" s="2"/>
-      <c r="F258" s="10"/>
-    </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="42">
-        <v>191</v>
-      </c>
-      <c r="B259" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="C259" s="11"/>
-      <c r="D259" s="11"/>
-      <c r="E259" s="11"/>
-      <c r="F259" s="12"/>
+      <c r="C256" s="11"/>
+      <c r="D256" s="11"/>
+      <c r="E256" s="11"/>
+      <c r="F256" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A244:F244"/>
-    <mergeCell ref="A250:F250"/>
-    <mergeCell ref="A255:F255"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A128:F128"/>
+    <mergeCell ref="A180:F180"/>
+    <mergeCell ref="A157:F157"/>
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="A111:F111"/>
+    <mergeCell ref="A121:F121"/>
+    <mergeCell ref="A165:F165"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A241:F241"/>
+    <mergeCell ref="A247:F247"/>
+    <mergeCell ref="A252:F252"/>
     <mergeCell ref="A64:F64"/>
     <mergeCell ref="A69:F69"/>
     <mergeCell ref="A77:F77"/>
@@ -4949,22 +4913,11 @@
     <mergeCell ref="A98:F98"/>
     <mergeCell ref="A102:F102"/>
     <mergeCell ref="A124:F124"/>
-    <mergeCell ref="A223:F223"/>
+    <mergeCell ref="A220:F220"/>
     <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A157:F157"/>
     <mergeCell ref="A154:F154"/>
-    <mergeCell ref="A233:F233"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A128:F128"/>
-    <mergeCell ref="A183:F183"/>
-    <mergeCell ref="A160:F160"/>
-    <mergeCell ref="A106:F106"/>
-    <mergeCell ref="A111:F111"/>
-    <mergeCell ref="A121:F121"/>
-    <mergeCell ref="A168:F168"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A151:F151"/>
+    <mergeCell ref="A230:F230"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>